<commit_message>
Adding a row in table II of paper.
</commit_message>
<xml_diff>
--- a/test_result/Test result single run imbalanced dataset.xlsx
+++ b/test_result/Test result single run imbalanced dataset.xlsx
@@ -1,19 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20379"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\huangfu\time-sequence-alchemy-notebook\test_result\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC35C24E-F1FB-4B0A-8DB4-49708051AA87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19176" windowHeight="6288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Summary" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="ts-120" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="multiple-ts" sheetId="3" r:id="rId6"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="ts-120" sheetId="2" r:id="rId2"/>
+    <sheet name="multiple-ts" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="62">
   <si>
     <t>The result from notebook #07 and after.</t>
   </si>
@@ -209,22 +218,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -234,70 +245,62 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="10" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -487,35 +490,40 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A2:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
@@ -529,28 +537,28 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="4">
         <f>'ts-120'!I10</f>
-        <v>0.999605</v>
+        <v>0.99960499999999997</v>
       </c>
       <c r="D7" s="4">
         <f>'ts-120'!J10</f>
-        <v>0.994574</v>
+        <v>0.99457399999999996</v>
       </c>
       <c r="E7" s="4">
         <f>'ts-120'!K10</f>
-        <v>0.999221</v>
+        <v>0.99922100000000003</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" ref="F7:F10" si="1">E7*D7*2/(D7+E7)</f>
-        <v>0.9968920845</v>
-      </c>
-    </row>
-    <row r="8">
+        <f t="shared" ref="F7:F10" si="0">E7*D7*2/(D7+E7)</f>
+        <v>0.99689208454630496</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
@@ -560,39 +568,39 @@
       </c>
       <c r="D8" s="4">
         <f>'ts-120'!J11</f>
-        <v>0.994569</v>
+        <v>0.99456900000000004</v>
       </c>
       <c r="E8" s="4">
         <f>'ts-120'!K11</f>
-        <v>0.998442</v>
+        <v>0.99844200000000005</v>
       </c>
       <c r="F8" s="4">
-        <f t="shared" si="1"/>
-        <v>0.9965017368</v>
-      </c>
-    </row>
-    <row r="9">
+        <f t="shared" si="0"/>
+        <v>0.99650173681730814</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="4">
         <f>'ts-120'!I12</f>
-        <v>0.997086</v>
+        <v>0.99708600000000003</v>
       </c>
       <c r="D9" s="4">
         <f>'ts-120'!J12</f>
-        <v>0.993554</v>
+        <v>0.99355400000000005</v>
       </c>
       <c r="E9" s="4">
         <f>'ts-120'!K12</f>
-        <v>0.96028</v>
+        <v>0.96028000000000002</v>
       </c>
       <c r="F9" s="4">
-        <f t="shared" si="1"/>
-        <v>0.9766336701</v>
-      </c>
-    </row>
-    <row r="10">
+        <f t="shared" si="0"/>
+        <v>0.97663367012755442</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -602,49 +610,49 @@
       </c>
       <c r="D10" s="4">
         <f>'ts-120'!J13</f>
-        <v>0.994569</v>
+        <v>0.99456900000000004</v>
       </c>
       <c r="E10" s="4">
         <f>'ts-120'!K13</f>
-        <v>0.998442</v>
+        <v>0.99844200000000005</v>
       </c>
       <c r="F10" s="4">
-        <f t="shared" si="1"/>
-        <v>0.9965017368</v>
-      </c>
-    </row>
-    <row r="11">
+        <f t="shared" si="0"/>
+        <v>0.99650173681730814</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="4">
         <f>'multiple-ts'!D27</f>
-        <v>0.996988</v>
+        <v>0.99698799999999999</v>
       </c>
       <c r="D11" s="4">
         <f>'multiple-ts'!E27</f>
-        <v>0.978108</v>
+        <v>0.97810799999999998</v>
       </c>
       <c r="E11" s="4">
         <f>'multiple-ts'!F27</f>
-        <v>0.974299</v>
+        <v>0.97429900000000003</v>
       </c>
       <c r="F11" s="4">
         <f>'multiple-ts'!G27</f>
-        <v>0.9762</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>0.97619999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="4">
         <f>'multiple-ts'!D22</f>
-        <v>0.998667</v>
+        <v>0.99866699999999997</v>
       </c>
       <c r="D12" s="4">
         <f>'multiple-ts'!E22</f>
-        <v>0.979405</v>
+        <v>0.97940499999999997</v>
       </c>
       <c r="E12" s="4">
         <f>'multiple-ts'!F22</f>
@@ -655,12 +663,12 @@
         <v>0.989595</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="3"/>
       <c r="E15" s="1" t="s">
@@ -676,7 +684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
@@ -705,15 +713,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="1">
-        <v>101245.0</v>
+        <v>101245</v>
       </c>
       <c r="D17" s="1">
-        <v>6422.0</v>
+        <v>6422</v>
       </c>
       <c r="E17" s="5">
         <f>'multiple-ts'!D2</f>
@@ -725,147 +733,147 @@
       </c>
       <c r="G17" s="5">
         <f>'multiple-ts'!D3</f>
-        <v>0.999605</v>
+        <v>0.99960499999999997</v>
       </c>
       <c r="H17" s="5">
         <f>'multiple-ts'!D5</f>
-        <v>0.997086</v>
+        <v>0.99708600000000003</v>
       </c>
       <c r="I17" s="5">
         <f>'multiple-ts'!D27</f>
-        <v>0.996988</v>
+        <v>0.99698799999999999</v>
       </c>
       <c r="J17" s="5">
         <f>'multiple-ts'!D22</f>
-        <v>0.998667</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>0.99866699999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="1">
-        <v>106560.0</v>
+        <v>106560</v>
       </c>
       <c r="D18" s="1">
-        <v>6510.0</v>
+        <v>6510</v>
       </c>
       <c r="E18" s="4">
         <f>'multiple-ts'!D10</f>
-        <v>0.99838596</v>
+        <v>0.99838596000000002</v>
       </c>
       <c r="F18" s="4">
         <f>'multiple-ts'!D8</f>
-        <v>0.999155</v>
+        <v>0.99915500000000002</v>
       </c>
       <c r="G18" s="4">
         <f>'multiple-ts'!D7</f>
-        <v>0.997372</v>
+        <v>0.99737200000000004</v>
       </c>
       <c r="H18" s="4">
         <f>'multiple-ts'!D9</f>
-        <v>0.993994</v>
+        <v>0.99399400000000004</v>
       </c>
       <c r="I18" s="5">
         <f>'multiple-ts'!D28</f>
-        <v>0.996997</v>
+        <v>0.99699700000000002</v>
       </c>
       <c r="J18" s="5">
         <f>'multiple-ts'!D23</f>
-        <v>0.999155</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>0.99915500000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="1">
-        <v>120811.0</v>
+        <v>120811</v>
       </c>
       <c r="D19" s="1">
-        <v>6805.0</v>
+        <v>6805</v>
       </c>
       <c r="E19" s="4">
         <f>'multiple-ts'!D10</f>
-        <v>0.99838596</v>
+        <v>0.99838596000000002</v>
       </c>
       <c r="F19" s="4">
         <f>'multiple-ts'!D12</f>
-        <v>0.99892397</v>
+        <v>0.99892396999999999</v>
       </c>
       <c r="G19" s="4">
         <f>'multiple-ts'!D11</f>
-        <v>0.99515789</v>
+        <v>0.99515788999999999</v>
       </c>
       <c r="H19" s="4">
         <f>'multiple-ts'!D13</f>
-        <v>0.990978</v>
+        <v>0.99097800000000003</v>
       </c>
       <c r="I19" s="5">
         <f>'multiple-ts'!D29</f>
-        <v>0.995034</v>
+        <v>0.99503399999999997</v>
       </c>
       <c r="J19" s="5">
         <f>'multiple-ts'!D24</f>
-        <v>0.998883</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>0.99888299999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="1">
-        <v>138179.0</v>
+        <v>138179</v>
       </c>
       <c r="D20" s="1">
-        <v>7064.0</v>
+        <v>7064</v>
       </c>
       <c r="E20" s="4">
         <f>'multiple-ts'!D14</f>
-        <v>0.996092</v>
+        <v>0.99609199999999998</v>
       </c>
       <c r="F20" s="4">
         <f>'multiple-ts'!D16</f>
-        <v>0.998806</v>
+        <v>0.99880599999999997</v>
       </c>
       <c r="G20" s="4">
         <f>'multiple-ts'!D15</f>
-        <v>0.993885</v>
+        <v>0.99388500000000002</v>
       </c>
       <c r="H20" s="4">
         <f>'multiple-ts'!D17</f>
-        <v>0.995622</v>
+        <v>0.99562200000000001</v>
       </c>
       <c r="I20" s="5">
         <f>'multiple-ts'!D30</f>
-        <v>0.994391</v>
+        <v>0.99439100000000002</v>
       </c>
       <c r="J20" s="5">
         <f>'multiple-ts'!D25</f>
-        <v>0.998842</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>0.99884200000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="1">
-        <v>167661.0</v>
+        <v>167661</v>
       </c>
       <c r="D21" s="1">
-        <v>7393.0</v>
+        <v>7393</v>
       </c>
       <c r="E21" s="4">
         <f>'multiple-ts'!D18</f>
-        <v>0.995557</v>
+        <v>0.99555700000000003</v>
       </c>
       <c r="F21" s="4">
         <f>'multiple-ts'!D20</f>
-        <v>0.998569</v>
+        <v>0.99856900000000004</v>
       </c>
       <c r="G21" s="4">
         <f>'multiple-ts'!D19</f>
-        <v>0.993231</v>
+        <v>0.99323099999999998</v>
       </c>
       <c r="H21" s="4">
         <f>'multiple-ts'!D21</f>
@@ -873,14 +881,14 @@
       </c>
       <c r="I21" s="5">
         <f>'multiple-ts'!D31</f>
-        <v>0.993439</v>
+        <v>0.99343899999999996</v>
       </c>
       <c r="J21" s="5">
         <f>'multiple-ts'!D26</f>
-        <v>0.998569</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>0.99856900000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="3"/>
       <c r="E23" s="1" t="s">
@@ -896,7 +904,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
@@ -925,15 +933,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C25" s="1">
-        <v>101245.0</v>
+        <v>101245</v>
       </c>
       <c r="D25" s="1">
-        <v>6422.0</v>
+        <v>6422</v>
       </c>
       <c r="E25" s="5">
         <f>'multiple-ts'!G2</f>
@@ -941,7 +949,7 @@
       </c>
       <c r="F25" s="5">
         <f>'multiple-ts'!G4</f>
-        <v>0.996505</v>
+        <v>0.99650499999999997</v>
       </c>
       <c r="G25" s="5">
         <f>'multiple-ts'!G3</f>
@@ -953,57 +961,57 @@
       </c>
       <c r="I25" s="5">
         <f>'multiple-ts'!G27</f>
-        <v>0.9762</v>
+        <v>0.97619999999999996</v>
       </c>
       <c r="J25" s="5">
         <f>'multiple-ts'!G22</f>
         <v>0.989595</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="1">
-        <v>106560.0</v>
+        <v>106560</v>
       </c>
       <c r="D26" s="1">
-        <v>6510.0</v>
+        <v>6510</v>
       </c>
       <c r="E26" s="5">
         <f>'multiple-ts'!G6</f>
-        <v>0.988986</v>
+        <v>0.98898600000000003</v>
       </c>
       <c r="F26" s="5">
         <f>'multiple-ts'!G8</f>
-        <v>0.993135</v>
+        <v>0.99313499999999999</v>
       </c>
       <c r="G26" s="5">
         <f>'multiple-ts'!G7</f>
-        <v>0.978022</v>
+        <v>0.97802199999999995</v>
       </c>
       <c r="H26" s="5">
         <f>'multiple-ts'!G9</f>
-        <v>0.951405</v>
+        <v>0.95140499999999995</v>
       </c>
       <c r="I26" s="5">
         <f>'multiple-ts'!G28</f>
-        <v>0.975366</v>
+        <v>0.97536599999999996</v>
       </c>
       <c r="J26" s="5">
         <f>'multiple-ts'!G23</f>
-        <v>0.993135</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>0.99313499999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C27" s="1">
-        <v>120811.0</v>
+        <v>120811</v>
       </c>
       <c r="D27" s="1">
-        <v>6805.0</v>
+        <v>6805</v>
       </c>
       <c r="E27" s="5">
         <f>'multiple-ts'!G10</f>
@@ -1011,15 +1019,15 @@
       </c>
       <c r="F27" s="5">
         <f>'multiple-ts'!G12</f>
-        <v>0.99053168</v>
+        <v>0.99053168000000003</v>
       </c>
       <c r="G27" s="5">
         <f>'multiple-ts'!G11</f>
-        <v>0.95508637</v>
+        <v>0.95508636999999996</v>
       </c>
       <c r="H27" s="5">
         <f>'multiple-ts'!G13</f>
-        <v>0.920205</v>
+        <v>0.92020500000000005</v>
       </c>
       <c r="I27" s="5">
         <f>'multiple-ts'!G29</f>
@@ -1027,69 +1035,69 @@
       </c>
       <c r="J27" s="5">
         <f>'multiple-ts'!G24</f>
-        <v>0.990164</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>0.99016400000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C28" s="1">
-        <v>138179.0</v>
+        <v>138179</v>
       </c>
       <c r="D28" s="1">
-        <v>7064.0</v>
+        <v>7064</v>
       </c>
       <c r="E28" s="5">
         <f>'multiple-ts'!G14</f>
-        <v>0.963165</v>
+        <v>0.96316500000000005</v>
       </c>
       <c r="F28" s="5">
         <f>'multiple-ts'!G16</f>
-        <v>0.988441</v>
+        <v>0.98844100000000001</v>
       </c>
       <c r="G28" s="5">
         <f>'multiple-ts'!G15</f>
-        <v>0.936394</v>
+        <v>0.93639399999999995</v>
       </c>
       <c r="H28" s="5">
         <f>'multiple-ts'!G17</f>
-        <v>0.9554</v>
+        <v>0.95540000000000003</v>
       </c>
       <c r="I28" s="5">
         <f>'multiple-ts'!G30</f>
-        <v>0.942099</v>
+        <v>0.94209900000000002</v>
       </c>
       <c r="J28" s="5">
         <f>'multiple-ts'!G25</f>
-        <v>0.988796</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>0.98879600000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C29" s="1">
-        <v>167661.0</v>
+        <v>167661</v>
       </c>
       <c r="D29" s="1">
-        <v>7393.0</v>
+        <v>7393</v>
       </c>
       <c r="E29" s="5">
         <f>'multiple-ts'!G18</f>
-        <v>0.951858</v>
+        <v>0.95185799999999998</v>
       </c>
       <c r="F29" s="5">
         <f>'multiple-ts'!G20</f>
-        <v>0.984021</v>
+        <v>0.98402100000000003</v>
       </c>
       <c r="G29" s="5">
         <f>'multiple-ts'!G19</f>
-        <v>0.91688</v>
+        <v>0.91688000000000003</v>
       </c>
       <c r="H29" s="5">
         <f>'multiple-ts'!G21</f>
-        <v>0.9278975741</v>
+        <v>0.92789757409999996</v>
       </c>
       <c r="I29" s="5">
         <f>'multiple-ts'!G31</f>
@@ -1097,38 +1105,182 @@
       </c>
       <c r="J29" s="5">
         <f>'multiple-ts'!G26</f>
-        <v>0.984021</v>
-      </c>
+        <v>0.98402100000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34">
+        <v>101245</v>
+      </c>
+      <c r="D34" s="12">
+        <f>'multiple-ts'!E4</f>
+        <v>0.99380299999999999</v>
+      </c>
+      <c r="E34" s="12">
+        <f>'multiple-ts'!F4</f>
+        <v>0.99922100000000003</v>
+      </c>
+      <c r="F34" s="12">
+        <f>'multiple-ts'!G4</f>
+        <v>0.99650499999999997</v>
+      </c>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+    </row>
+    <row r="35" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35">
+        <v>106560</v>
+      </c>
+      <c r="D35" s="12">
+        <f>'multiple-ts'!E8</f>
+        <v>0.98636400000000002</v>
+      </c>
+      <c r="E35" s="12">
+        <f>'multiple-ts'!F8</f>
+        <v>1</v>
+      </c>
+      <c r="F35" s="12">
+        <f>'multiple-ts'!G8</f>
+        <v>0.99313499999999999</v>
+      </c>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+    </row>
+    <row r="36" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36">
+        <v>120811</v>
+      </c>
+      <c r="D36" s="12">
+        <f>'multiple-ts'!E12</f>
+        <v>0.98194946000000005</v>
+      </c>
+      <c r="E36" s="12">
+        <f>'multiple-ts'!F12</f>
+        <v>0.99926524999999999</v>
+      </c>
+      <c r="F36" s="12">
+        <f>'multiple-ts'!G12</f>
+        <v>0.99053168000000003</v>
+      </c>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+    </row>
+    <row r="37" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37">
+        <v>138179</v>
+      </c>
+      <c r="D37" s="12">
+        <f>'multiple-ts'!E16</f>
+        <v>0.97850199999999998</v>
+      </c>
+      <c r="E37" s="12">
+        <f>'multiple-ts'!F16</f>
+        <v>0.99858499999999994</v>
+      </c>
+      <c r="F37" s="12">
+        <f>'multiple-ts'!G16</f>
+        <v>0.98844100000000001</v>
+      </c>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+    </row>
+    <row r="38" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38">
+        <v>167661</v>
+      </c>
+      <c r="D38" s="12">
+        <f>'multiple-ts'!E20</f>
+        <v>0.96918000000000004</v>
+      </c>
+      <c r="E38" s="12">
+        <f>'multiple-ts'!F20</f>
+        <v>0.99932399999999999</v>
+      </c>
+      <c r="F38" s="12">
+        <f>'multiple-ts'!G20</f>
+        <v>0.98402100000000003</v>
+      </c>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="3.71"/>
-    <col customWidth="1" min="2" max="2" width="9.57"/>
-    <col customWidth="1" min="3" max="3" width="14.57"/>
-    <col customWidth="1" min="4" max="4" width="9.14"/>
-    <col customWidth="1" min="5" max="5" width="9.86"/>
-    <col customWidth="1" min="6" max="6" width="7.43"/>
-    <col customWidth="1" min="7" max="7" width="8.86"/>
-    <col customWidth="1" min="8" max="8" width="9.29"/>
-    <col customWidth="1" min="9" max="9" width="12.29"/>
-    <col customWidth="1" min="10" max="10" width="8.71"/>
-    <col customWidth="1" min="11" max="11" width="9.57"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1157,38 +1309,38 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>120.0</v>
+        <v>120</v>
       </c>
       <c r="C2" s="1">
-        <v>101245.0</v>
+        <v>101245</v>
       </c>
       <c r="D2" s="1">
-        <v>6422.0</v>
+        <v>6422</v>
       </c>
       <c r="E2" s="4">
         <f>D2/C2</f>
-        <v>0.06343029285</v>
+        <v>6.3430292853968104E-2</v>
       </c>
       <c r="F2" s="7">
-        <v>64796.0</v>
+        <v>64796</v>
       </c>
       <c r="G2" s="7">
-        <v>16200.0</v>
+        <v>16200</v>
       </c>
       <c r="H2" s="8">
         <f>C2*0.2</f>
         <v>20249</v>
       </c>
       <c r="I2" s="1">
-        <v>121372.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>121372</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1226,7 +1378,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>44</v>
       </c>
@@ -1234,13 +1386,13 @@
         <v>45</v>
       </c>
       <c r="D5" s="9">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="E5" s="10">
-        <v>0.503195</v>
+        <v>0.50319499999999995</v>
       </c>
       <c r="F5" s="11">
-        <v>0.999878</v>
+        <v>0.99987800000000004</v>
       </c>
       <c r="G5" s="11">
         <v>0.999027</v>
@@ -1249,19 +1401,19 @@
         <v>0.999027</v>
       </c>
       <c r="I5" s="11">
-        <v>0.999463</v>
+        <v>0.99946299999999999</v>
       </c>
       <c r="J5" s="11">
-        <v>0.993029</v>
+        <v>0.99302900000000005</v>
       </c>
       <c r="K5" s="11">
-        <v>0.998442</v>
+        <v>0.99844200000000005</v>
       </c>
       <c r="L5" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1269,34 +1421,34 @@
         <v>47</v>
       </c>
       <c r="D6" s="9">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="E6" s="10">
-        <v>0.506935</v>
+        <v>0.50693500000000002</v>
       </c>
       <c r="F6" s="11">
-        <v>0.998596</v>
+        <v>0.99859600000000004</v>
       </c>
       <c r="G6" s="11">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="11">
         <v>0.977626</v>
       </c>
       <c r="I6" s="11">
-        <v>0.997998</v>
+        <v>0.99799800000000005</v>
       </c>
       <c r="J6" s="11">
-        <v>0.998396</v>
+        <v>0.99839599999999995</v>
       </c>
       <c r="K6" s="11">
-        <v>0.969626</v>
+        <v>0.96962599999999999</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1304,117 +1456,117 @@
         <v>49</v>
       </c>
       <c r="D7" s="9">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="E7" s="10">
-        <v>0.50313</v>
+        <v>0.50312999999999997</v>
       </c>
       <c r="F7" s="11">
-        <v>0.999878</v>
+        <v>0.99987800000000004</v>
       </c>
       <c r="G7" s="11">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="11">
-        <v>0.998055</v>
+        <v>0.99805500000000003</v>
       </c>
       <c r="I7" s="11">
-        <v>0.999609</v>
+        <v>0.99960899999999997</v>
       </c>
       <c r="J7" s="11">
-        <v>0.995342</v>
+        <v>0.99534199999999995</v>
       </c>
       <c r="K7" s="11">
-        <v>0.998442</v>
+        <v>0.99844200000000005</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="9">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="E8" s="10">
-        <v>0.508095</v>
+        <v>0.50809499999999996</v>
       </c>
       <c r="F8" s="11">
         <v>0.998108</v>
       </c>
       <c r="G8" s="11">
-        <v>0.994054</v>
+        <v>0.99405399999999999</v>
       </c>
       <c r="H8" s="11">
-        <v>0.975681</v>
+        <v>0.97568100000000002</v>
       </c>
       <c r="I8" s="11">
-        <v>0.997998</v>
+        <v>0.99799800000000005</v>
       </c>
       <c r="J8" s="11">
-        <v>0.993646</v>
+        <v>0.99364600000000003</v>
       </c>
       <c r="K8" s="11">
-        <v>0.974299</v>
+        <v>0.97429900000000003</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="9">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="E9" s="10">
-        <v>0.503411</v>
+        <v>0.50341100000000005</v>
       </c>
       <c r="F9" s="11">
-        <v>0.99884</v>
+        <v>0.99883999999999995</v>
       </c>
       <c r="G9" s="11">
-        <v>0.981853</v>
+        <v>0.98185299999999998</v>
       </c>
       <c r="H9" s="11">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="11">
-        <v>0.998682</v>
+        <v>0.99868199999999996</v>
       </c>
       <c r="J9" s="11">
-        <v>0.979405</v>
+        <v>0.97940499999999997</v>
       </c>
       <c r="K9" s="11">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I10" s="11">
-        <v>0.999605</v>
+        <v>0.99960499999999997</v>
       </c>
       <c r="J10" s="11">
-        <v>0.994574</v>
+        <v>0.99457399999999996</v>
       </c>
       <c r="K10" s="11">
-        <v>0.999221</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>0.99922100000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
@@ -1428,15 +1580,15 @@
         <v>0.999556</v>
       </c>
       <c r="J11" s="11">
-        <v>0.994569</v>
+        <v>0.99456900000000004</v>
       </c>
       <c r="K11" s="11">
-        <v>0.998442</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>0.99844200000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>18</v>
@@ -1447,18 +1599,18 @@
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11">
-        <v>0.997086</v>
+        <v>0.99708600000000003</v>
       </c>
       <c r="J12" s="11">
-        <v>0.993554</v>
+        <v>0.99355400000000005</v>
       </c>
       <c r="K12" s="11">
-        <v>0.96028</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>0.96028000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>17</v>
@@ -1472,13 +1624,13 @@
         <v>0.999556</v>
       </c>
       <c r="J13" s="11">
-        <v>0.994569</v>
+        <v>0.99456900000000004</v>
       </c>
       <c r="K13" s="11">
-        <v>0.998442</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>0.99844200000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D14" s="9"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -1488,7 +1640,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D15" s="9"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
@@ -1498,7 +1650,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D16" s="9"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
@@ -1508,7 +1660,7 @@
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
     </row>
-    <row r="17">
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D17" s="9"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
@@ -1518,7 +1670,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
     </row>
-    <row r="18">
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D18" s="9"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
@@ -1528,7 +1680,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
     </row>
-    <row r="19">
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D19" s="9"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
@@ -1538,7 +1690,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
     </row>
-    <row r="20">
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
@@ -1548,24 +1700,27 @@
       <c r="K20" s="11"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.43"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -1588,697 +1743,697 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1">
-        <v>120.0</v>
+        <v>120</v>
       </c>
       <c r="D2" s="3">
         <v>0.999556</v>
       </c>
       <c r="E2" s="3">
-        <v>0.994569</v>
+        <v>0.99456900000000004</v>
       </c>
       <c r="F2" s="3">
-        <v>0.998442</v>
+        <v>0.99844200000000005</v>
       </c>
       <c r="G2" s="3">
         <v>0.996502</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1">
-        <v>120.0</v>
+        <v>120</v>
       </c>
       <c r="D3" s="3">
-        <v>0.999605</v>
+        <v>0.99960499999999997</v>
       </c>
       <c r="E3" s="3">
-        <v>0.994574</v>
+        <v>0.99457399999999996</v>
       </c>
       <c r="F3" s="3">
-        <v>0.999221</v>
+        <v>0.99922100000000003</v>
       </c>
       <c r="G3" s="3">
         <v>0.996892</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="1">
-        <v>120.0</v>
+        <v>120</v>
       </c>
       <c r="D4" s="3">
         <v>0.999556</v>
       </c>
       <c r="E4" s="3">
-        <v>0.993803</v>
+        <v>0.99380299999999999</v>
       </c>
       <c r="F4" s="3">
-        <v>0.999221</v>
+        <v>0.99922100000000003</v>
       </c>
       <c r="G4" s="3">
-        <v>0.996505</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>0.99650499999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="1">
-        <v>120.0</v>
+        <v>120</v>
       </c>
       <c r="D5" s="3">
-        <v>0.997086</v>
+        <v>0.99708600000000003</v>
       </c>
       <c r="E5" s="3">
-        <v>0.993554</v>
+        <v>0.99355400000000005</v>
       </c>
       <c r="F5" s="3">
-        <v>0.96028</v>
+        <v>0.96028000000000002</v>
       </c>
       <c r="G5" s="3">
         <v>0.976634</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>94.0</v>
+        <v>94</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="D6" s="3">
-        <v>0.998639</v>
+        <v>0.99863900000000005</v>
       </c>
       <c r="E6" s="3">
-        <v>0.978212</v>
+        <v>0.97821199999999997</v>
       </c>
       <c r="F6" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="3">
-        <v>0.988986</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>0.98898600000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="D7" s="3">
-        <v>0.997372</v>
+        <v>0.99737200000000004</v>
       </c>
       <c r="E7" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="3">
-        <v>0.956989</v>
+        <v>0.95698899999999998</v>
       </c>
       <c r="G7" s="3">
-        <v>0.978022</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>0.97802199999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>113.0</v>
+        <v>113</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="1">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="D8" s="3">
-        <v>0.999155</v>
+        <v>0.99915500000000002</v>
       </c>
       <c r="E8" s="3">
-        <v>0.986364</v>
+        <v>0.98636400000000002</v>
       </c>
       <c r="F8" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="3">
-        <v>0.993135</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>0.99313499999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>129.0</v>
+        <v>129</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="1">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="D9" s="3">
-        <v>0.993994</v>
+        <v>0.99399400000000004</v>
       </c>
       <c r="E9" s="3">
-        <v>0.940691</v>
+        <v>0.94069100000000005</v>
       </c>
       <c r="F9" s="3">
-        <v>0.962366</v>
+        <v>0.96236600000000005</v>
       </c>
       <c r="G9" s="3">
-        <v>0.951405</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>0.95140499999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>131.0</v>
+        <v>131</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="1">
-        <v>480.0</v>
+        <v>480</v>
       </c>
       <c r="D10" s="3">
-        <v>0.99838596</v>
+        <v>0.99838596000000002</v>
       </c>
       <c r="E10" s="3">
-        <v>0.97214286</v>
+        <v>0.97214286000000005</v>
       </c>
       <c r="F10" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="3">
         <v>0.98587468</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>152.0</v>
+        <v>152</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1">
-        <v>480.0</v>
+        <v>480</v>
       </c>
       <c r="D11" s="3">
-        <v>0.99515789</v>
+        <v>0.99515788999999999</v>
       </c>
       <c r="E11" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="3">
-        <v>0.9140338</v>
+        <v>0.91403380000000001</v>
       </c>
       <c r="G11" s="3">
-        <v>0.95508637</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>0.95508636999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>141.0</v>
+        <v>141</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="1">
-        <v>480.0</v>
+        <v>480</v>
       </c>
       <c r="D12" s="3">
-        <v>0.99892397</v>
+        <v>0.99892396999999999</v>
       </c>
       <c r="E12" s="3">
-        <v>0.98194946</v>
+        <v>0.98194946000000005</v>
       </c>
       <c r="F12" s="3">
-        <v>0.99926525</v>
+        <v>0.99926524999999999</v>
       </c>
       <c r="G12" s="3">
-        <v>0.99053168</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>0.99053168000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>164.0</v>
+        <v>164</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C13" s="1">
-        <v>480.0</v>
+        <v>480</v>
       </c>
       <c r="D13" s="3">
-        <v>0.990978</v>
+        <v>0.99097800000000003</v>
       </c>
       <c r="E13" s="3">
-        <v>0.916849</v>
+        <v>0.91684900000000003</v>
       </c>
       <c r="F13" s="3">
-        <v>0.923586</v>
+        <v>0.92358600000000002</v>
       </c>
       <c r="G13" s="3">
-        <v>0.920205</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>0.92020500000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>175.0</v>
+        <v>175</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="1">
-        <v>960.0</v>
+        <v>960</v>
       </c>
       <c r="D14" s="3">
-        <v>0.996092</v>
+        <v>0.99609199999999998</v>
       </c>
       <c r="E14" s="3">
-        <v>0.929559</v>
+        <v>0.92955900000000002</v>
       </c>
       <c r="F14" s="3">
-        <v>0.999292</v>
+        <v>0.99929199999999996</v>
       </c>
       <c r="G14" s="3">
-        <v>0.963165</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>0.96316500000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>181.0</v>
+        <v>181</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>960.0</v>
+        <v>960</v>
       </c>
       <c r="D15" s="3">
-        <v>0.993885</v>
+        <v>0.99388500000000002</v>
       </c>
       <c r="E15" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="3">
-        <v>0.880396</v>
+        <v>0.88039599999999996</v>
       </c>
       <c r="G15" s="3">
-        <v>0.936394</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>0.93639399999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>196.0</v>
+        <v>196</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="1">
-        <v>960.0</v>
+        <v>960</v>
       </c>
       <c r="D16" s="3">
-        <v>0.998806</v>
+        <v>0.99880599999999997</v>
       </c>
       <c r="E16" s="3">
-        <v>0.978502</v>
+        <v>0.97850199999999998</v>
       </c>
       <c r="F16" s="3">
-        <v>0.998585</v>
+        <v>0.99858499999999994</v>
       </c>
       <c r="G16" s="3">
-        <v>0.988441</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>0.98844100000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>205.0</v>
+        <v>205</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C17" s="1">
-        <v>960.0</v>
+        <v>960</v>
       </c>
       <c r="D17" s="3">
-        <v>0.995622</v>
+        <v>0.99562200000000001</v>
       </c>
       <c r="E17" s="3">
         <v>0.996923</v>
       </c>
       <c r="F17" s="3">
-        <v>0.917197</v>
+        <v>0.91719700000000004</v>
       </c>
       <c r="G17" s="3">
-        <v>0.9554</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>0.95540000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>212.0</v>
+        <v>212</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="1">
-        <v>1920.0</v>
+        <v>1920</v>
       </c>
       <c r="D18" s="3">
-        <v>0.995557</v>
+        <v>0.99555700000000003</v>
       </c>
       <c r="E18" s="3">
-        <v>0.91151</v>
+        <v>0.91151000000000004</v>
       </c>
       <c r="F18" s="3">
-        <v>0.995943</v>
+        <v>0.99594300000000002</v>
       </c>
       <c r="G18" s="3">
-        <v>0.951858</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>0.95185799999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>229.0</v>
+        <v>229</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="1">
-        <v>1920.0</v>
+        <v>1920</v>
       </c>
       <c r="D19" s="3">
-        <v>0.993231</v>
+        <v>0.99323099999999998</v>
       </c>
       <c r="E19" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="3">
-        <v>0.846518</v>
+        <v>0.84651799999999999</v>
       </c>
       <c r="G19" s="3">
-        <v>0.91688</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>0.91688000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>236.0</v>
+        <v>236</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="1">
-        <v>1920.0</v>
+        <v>1920</v>
       </c>
       <c r="D20" s="3">
-        <v>0.998569</v>
+        <v>0.99856900000000004</v>
       </c>
       <c r="E20" s="3">
-        <v>0.96918</v>
+        <v>0.96918000000000004</v>
       </c>
       <c r="F20" s="3">
-        <v>0.999324</v>
+        <v>0.99932399999999999</v>
       </c>
       <c r="G20" s="3">
-        <v>0.984021</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>0.98402100000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>248.0</v>
+        <v>248</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C21" s="1">
-        <v>1920.0</v>
+        <v>1920</v>
       </c>
       <c r="D21" s="1">
         <v>0.9936182268</v>
       </c>
       <c r="E21" s="1">
-        <v>0.9247817327</v>
+        <v>0.92478173269999997</v>
       </c>
       <c r="F21" s="1">
-        <v>0.9310344828</v>
+        <v>0.93103448280000001</v>
       </c>
       <c r="G21" s="1">
-        <v>0.9278975741</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>0.92789757409999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>260.0</v>
+        <v>260</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C22" s="1">
-        <v>120.0</v>
+        <v>120</v>
       </c>
       <c r="D22" s="3">
-        <v>0.998667</v>
+        <v>0.99866699999999997</v>
       </c>
       <c r="E22" s="3">
-        <v>0.979405</v>
+        <v>0.97940499999999997</v>
       </c>
       <c r="F22" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="3">
         <v>0.989595</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>262.0</v>
+        <v>262</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C23" s="1">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="D23" s="3">
-        <v>0.999155</v>
+        <v>0.99915500000000002</v>
       </c>
       <c r="E23" s="3">
-        <v>0.986364</v>
+        <v>0.98636400000000002</v>
       </c>
       <c r="F23" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="3">
-        <v>0.993135</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>0.99313499999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>272.0</v>
+        <v>272</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C24" s="1">
-        <v>480.0</v>
+        <v>480</v>
       </c>
       <c r="D24" s="3">
-        <v>0.998883</v>
+        <v>0.99888299999999997</v>
       </c>
       <c r="E24" s="3">
-        <v>0.981936</v>
+        <v>0.98193600000000003</v>
       </c>
       <c r="F24" s="3">
-        <v>0.99853</v>
+        <v>0.99853000000000003</v>
       </c>
       <c r="G24" s="3">
-        <v>0.990164</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>0.99016400000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>285.0</v>
+        <v>285</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C25" s="1">
-        <v>960.0</v>
+        <v>960</v>
       </c>
       <c r="D25" s="3">
-        <v>0.998842</v>
+        <v>0.99884200000000001</v>
       </c>
       <c r="E25" s="3">
-        <v>0.978517</v>
+        <v>0.97851699999999997</v>
       </c>
       <c r="F25" s="3">
-        <v>0.999292</v>
+        <v>0.99929199999999996</v>
       </c>
       <c r="G25" s="3">
-        <v>0.988796</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>0.98879600000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>294.0</v>
+        <v>294</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C26" s="1">
-        <v>1920.0</v>
+        <v>1920</v>
       </c>
       <c r="D26" s="3">
-        <v>0.998569</v>
+        <v>0.99856900000000004</v>
       </c>
       <c r="E26" s="3">
-        <v>0.96918</v>
+        <v>0.96918000000000004</v>
       </c>
       <c r="F26" s="3">
-        <v>0.999324</v>
+        <v>0.99932399999999999</v>
       </c>
       <c r="G26" s="3">
-        <v>0.984021</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>0.98402100000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>305.0</v>
+        <v>305</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C27" s="1">
-        <v>120.0</v>
+        <v>120</v>
       </c>
       <c r="D27" s="3">
-        <v>0.996988</v>
+        <v>0.99698799999999999</v>
       </c>
       <c r="E27" s="3">
-        <v>0.978108</v>
+        <v>0.97810799999999998</v>
       </c>
       <c r="F27" s="3">
-        <v>0.974299</v>
+        <v>0.97429900000000003</v>
       </c>
       <c r="G27" s="3">
-        <v>0.9762</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>0.97619999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>320.0</v>
+        <v>320</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C28" s="1">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="D28" s="3">
-        <v>0.996997</v>
+        <v>0.99699700000000002</v>
       </c>
       <c r="E28" s="3">
-        <v>0.977623</v>
+        <v>0.97762300000000002</v>
       </c>
       <c r="F28" s="3">
-        <v>0.973118</v>
+        <v>0.97311800000000004</v>
       </c>
       <c r="G28" s="3">
-        <v>0.975366</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>0.97536599999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>322.0</v>
+        <v>322</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C29" s="1">
-        <v>480.0</v>
+        <v>480</v>
       </c>
       <c r="D29" s="3">
-        <v>0.995034</v>
+        <v>0.99503399999999997</v>
       </c>
       <c r="E29" s="3">
-        <v>0.99207</v>
+        <v>0.99207000000000001</v>
       </c>
       <c r="F29" s="3">
-        <v>0.919177</v>
+        <v>0.91917700000000002</v>
       </c>
       <c r="G29" s="3">
         <v>0.954233</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>332.0</v>
+        <v>332</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C30" s="1">
-        <v>960.0</v>
+        <v>960</v>
       </c>
       <c r="D30" s="3">
-        <v>0.994391</v>
+        <v>0.99439100000000002</v>
       </c>
       <c r="E30" s="3">
-        <v>0.997627</v>
+        <v>0.99762700000000004</v>
       </c>
       <c r="F30" s="3">
-        <v>0.892427</v>
+        <v>0.89242699999999997</v>
       </c>
       <c r="G30" s="3">
-        <v>0.942099</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>0.94209900000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>344.0</v>
+        <v>344</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C31" s="1">
-        <v>1920.0</v>
+        <v>1920</v>
       </c>
       <c r="D31" s="3">
-        <v>0.993439</v>
+        <v>0.99343899999999996</v>
       </c>
       <c r="E31" s="3">
-        <v>0.995279</v>
+        <v>0.99527900000000002</v>
       </c>
       <c r="F31" s="3">
-        <v>0.855308</v>
+        <v>0.85530799999999996</v>
       </c>
       <c r="G31" s="3">
         <v>0.92</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>